<commit_message>
Add new SEM BOT
</commit_message>
<xml_diff>
--- a/bot-list/elenco_bot.xlsx
+++ b/bot-list/elenco_bot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sasadangelo/github.com/sasadangelo/investire/bot-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C723C7-CFEE-9F40-87B7-00BA55D7DFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090E2523-95E1-0144-911B-5122E488027C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="2340" windowWidth="25600" windowHeight="14480" xr2:uid="{384A719B-2758-B34C-9A5E-16DC06482511}"/>
+    <workbookView xWindow="2820" yWindow="540" windowWidth="25600" windowHeight="14480" xr2:uid="{384A719B-2758-B34C-9A5E-16DC06482511}"/>
   </bookViews>
   <sheets>
     <sheet name="Elenco BOT" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>BOT</t>
   </si>
@@ -246,9 +246,6 @@
     <t>IT0005492415</t>
   </si>
   <si>
-    <t>IT0005508244</t>
-  </si>
-  <si>
     <t>IT0005529752</t>
   </si>
   <si>
@@ -291,10 +288,10 @@
     <t>IT0005518524</t>
   </si>
   <si>
-    <t>31/11/22</t>
-  </si>
-  <si>
-    <t>BOT 31MZ23 SEM</t>
+    <t>IT0005541278</t>
+  </si>
+  <si>
+    <t>BOT 29ST23 SEM</t>
   </si>
 </sst>
 </file>
@@ -359,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -374,6 +371,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +690,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="H3" sqref="H3:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +711,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>56</v>
@@ -727,15 +726,19 @@
         <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <f>F2-D2</f>
+        <v>366</v>
       </c>
       <c r="D2" s="2">
         <v>44999</v>
@@ -750,9 +753,9 @@
         <f t="shared" ref="G2:G17" si="0">100-E2</f>
         <v>3.5430000000000064</v>
       </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H17" si="1">ROUND(G2*100/E2,2)</f>
-        <v>3.67</v>
+      <c r="H2" s="11">
+        <f>(G2*100/E2)*(365/C2)</f>
+        <v>3.6631034265332265</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -762,6 +765,10 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C16" si="1">F3-D3</f>
+        <v>365</v>
+      </c>
       <c r="D3" s="2">
         <v>44971</v>
       </c>
@@ -775,18 +782,22 @@
         <f t="shared" si="0"/>
         <v>3.1230000000000047</v>
       </c>
-      <c r="H3">
-        <f t="shared" si="1"/>
-        <v>3.22</v>
+      <c r="H3" s="11">
+        <f t="shared" ref="H3:H17" si="2">(G3*100/E3)*(365/C3)</f>
+        <v>3.2236753821856632</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
       <c r="D4" s="2">
         <v>44939</v>
       </c>
@@ -800,18 +811,22 @@
         <f t="shared" si="0"/>
         <v>3.0259999999999962</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+      <c r="H4" s="11">
+        <f t="shared" si="2"/>
+        <v>3.1289966246758749</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D5" s="2">
         <v>44909</v>
       </c>
@@ -825,18 +840,22 @@
         <f t="shared" si="0"/>
         <v>2.6350000000000051</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>2.71</v>
+      <c r="H5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.7063113028295644</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D6" s="2">
         <v>44879</v>
       </c>
@@ -850,18 +869,22 @@
         <f t="shared" si="0"/>
         <v>2.6550000000000011</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>2.73</v>
+      <c r="H6" s="11">
+        <f t="shared" si="2"/>
+        <v>2.7274128101083788</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
       <c r="D7" s="2">
         <v>44848</v>
       </c>
@@ -875,9 +898,9 @@
         <f t="shared" si="0"/>
         <v>2.4959999999999951</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>2.56</v>
+      <c r="H7" s="11">
+        <f t="shared" si="2"/>
+        <v>2.5669276571803596</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -887,6 +910,10 @@
       <c r="B8" t="s">
         <v>50</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D8" s="2">
         <v>44818</v>
       </c>
@@ -900,9 +927,9 @@
         <f t="shared" si="0"/>
         <v>2.0759999999999934</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>2.12</v>
+      <c r="H8" s="11">
+        <f t="shared" si="2"/>
+        <v>2.1200114374412742</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -912,6 +939,10 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D9" s="2">
         <v>44787</v>
       </c>
@@ -925,9 +956,9 @@
         <f t="shared" si="0"/>
         <v>1.0030000000000001</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>1.01</v>
+      <c r="H9" s="11">
+        <f t="shared" si="2"/>
+        <v>1.013162015010556</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -937,6 +968,10 @@
       <c r="B10" t="s">
         <v>51</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D10" s="2">
         <v>44756</v>
       </c>
@@ -950,9 +985,9 @@
         <f t="shared" si="0"/>
         <v>0.72700000000000387</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>0.73</v>
+      <c r="H10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.73232399544690285</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -962,6 +997,10 @@
       <c r="B11" t="s">
         <v>52</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D11" s="2">
         <v>44726</v>
       </c>
@@ -975,9 +1014,9 @@
         <f t="shared" si="0"/>
         <v>0.89700000000000557</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>0.91</v>
+      <c r="H11" s="11">
+        <f t="shared" si="2"/>
+        <v>0.90511891668264899</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -987,6 +1026,10 @@
       <c r="B12" t="s">
         <v>53</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
       <c r="D12" s="2">
         <v>44694</v>
       </c>
@@ -1000,9 +1043,9 @@
         <f t="shared" si="0"/>
         <v>0.12199999999999989</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>0.12</v>
+      <c r="H12" s="11">
+        <f t="shared" si="2"/>
+        <v>0.12248459604233637</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1012,6 +1055,10 @@
       <c r="B13" t="s">
         <v>54</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
       <c r="D13" s="2">
         <v>44665</v>
       </c>
@@ -1025,121 +1072,125 @@
         <f t="shared" si="0"/>
         <v>0.30800000000000693</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>0.31</v>
+      <c r="H13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.30895157083818858</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="7">
-        <v>179</v>
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>182</v>
       </c>
       <c r="D14" s="2">
-        <v>44865</v>
+        <v>45016</v>
       </c>
       <c r="E14">
-        <v>98.991</v>
+        <v>98.468999999999994</v>
       </c>
       <c r="F14" s="2">
-        <v>45044</v>
+        <v>45198</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>1.0090000000000003</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>1.02</v>
+        <v>1.5310000000000059</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="2"/>
+        <v>3.1181509794068183</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15">
-        <v>181</v>
+        <f t="shared" si="1"/>
+        <v>179</v>
       </c>
       <c r="D15" s="2">
-        <v>44957</v>
+        <v>44865</v>
       </c>
       <c r="E15">
-        <v>98.600999999999999</v>
+        <v>98.991</v>
       </c>
       <c r="F15" s="2">
-        <v>45138</v>
+        <v>45044</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>1.3990000000000009</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>1.42</v>
+        <v>1.0090000000000003</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="2"/>
+        <v>2.078429453746967</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C16">
-        <v>182</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>83</v>
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+      <c r="D16" s="2">
+        <v>44957</v>
       </c>
       <c r="E16">
-        <v>98.838999999999999</v>
+        <v>98.600999999999999</v>
       </c>
       <c r="F16" s="2">
-        <v>45077</v>
+        <v>45138</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>1.1610000000000014</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>1.17</v>
+        <v>1.3990000000000009</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="2"/>
+        <v>2.8612162607923546</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="C17" s="10">
+        <f>F17-D17</f>
         <v>182</v>
       </c>
-      <c r="D17" s="2">
-        <v>44834</v>
+      <c r="D17" s="8">
+        <v>44895</v>
       </c>
       <c r="E17">
-        <v>99.01</v>
+        <v>98.838999999999999</v>
       </c>
       <c r="F17" s="2">
-        <v>45016</v>
+        <v>45077</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.98999999999999488</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1610000000000014</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="2"/>
+        <v>2.3557291361498232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>